<commit_message>
Update the chart we created
</commit_message>
<xml_diff>
--- a/awesome_security_repo.xlsx
+++ b/awesome_security_repo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VirtualShare\awesome-cybersecurity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95DEB49-2736-4B3F-A430-D2A136D6E4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30736B29-3413-487A-9973-2C75F08F5C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{81CE6068-20D0-4AC4-A877-CDE743AA0958}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81CE6068-20D0-4AC4-A877-CDE743AA0958}"/>
   </bookViews>
   <sheets>
     <sheet name="security" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="637">
   <si>
     <t>id</t>
   </si>
@@ -2090,7 +2090,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2103,10 +2103,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="1"/>
               <a:t>Top Repositories </a:t>
             </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1600" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2123,7 +2123,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2173,12 +2173,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="bg1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -2199,6 +2196,454 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="20"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="21"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="22"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="23"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="24"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="25"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="26"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="27"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="28"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="29"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="30"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="31"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="32"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -2233,6 +2678,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2248,6 +2698,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2263,6 +2718,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2278,6 +2738,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -2293,6 +2758,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -2308,6 +2778,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -2325,6 +2800,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -2342,6 +2822,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -2359,6 +2844,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -2376,6 +2866,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -2393,6 +2888,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -2410,6 +2910,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -2428,6 +2933,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -2446,6 +2956,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -2464,6 +2979,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -2482,6 +3002,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -2500,6 +3025,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -2518,6 +3048,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
@@ -2535,6 +3070,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="19"/>
@@ -2552,6 +3092,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="20"/>
@@ -2569,6 +3114,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="21"/>
@@ -2586,6 +3136,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="22"/>
@@ -2603,6 +3158,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002D-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="23"/>
@@ -2620,6 +3180,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002F-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="24"/>
@@ -2638,6 +3203,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="25"/>
@@ -2656,6 +3226,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000033-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="26"/>
@@ -2674,6 +3249,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000035-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="27"/>
@@ -2692,6 +3272,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000037-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="28"/>
@@ -2710,6 +3295,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000039-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="29"/>
@@ -2728,6 +3318,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003B-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="30"/>
@@ -2745,6 +3340,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003D-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="31"/>
@@ -2762,6 +3362,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003F-6AC8-41BB-B727-BCEE916DECE5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -2778,12 +3383,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="bg1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2821,9 +3423,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>graphic1!$A$4:$A$36</c:f>
+              <c:f>graphic1!$A$4:$A$18</c:f>
               <c:strCache>
-                <c:ptCount val="32"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Awesome-Hacking</c:v>
                 </c:pt>
@@ -2866,69 +3468,15 @@
                 <c:pt idx="13">
                   <c:v>awesome-api-security</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>awesome-golang-security</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>awesome-programming-books</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>awesome-game-security</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>awesome-windows-kernel-security-development</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>awesome-k8s-security</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>awesome-windows-domain-hardening</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>awesome-security-weixin-official-accounts</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>awesome-cyber-security</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>awesome-android-security</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>awesome-industrial-control-system-security</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>awesome-embedded-and-iot-security</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>awesome-java-security</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Awesome-AI-Security</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>awesome-ethereum-security</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>awesome-lockpicking</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>osx-and-ios-security-awesome</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Awesome-web3-Security</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>awesome-canbus</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>graphic1!$B$4:$B$36</c:f>
+              <c:f>graphic1!$B$4:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>64822</c:v>
                 </c:pt>
@@ -2971,60 +3519,6 @@
                 <c:pt idx="13">
                   <c:v>2139</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>1820</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1759</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1755</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1742</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1714</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1635</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1510</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1391</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1255</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1190</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1184</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1177</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1108</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1096</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1081</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1031</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1009</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3060,9 +3554,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.66187260125418457"/>
+          <c:x val="0.64505297502949743"/>
           <c:y val="0.18568633717833241"/>
-          <c:w val="0.31060451732524258"/>
+          <c:w val="0.32742408919068605"/>
           <c:h val="0.76324601893002952"/>
         </c:manualLayout>
       </c:layout>
@@ -3079,7 +3573,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3180,7 +3674,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3193,10 +3687,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="1"/>
               <a:t>Trend of Updated Awesome Security repositories</a:t>
             </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1600" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3213,7 +3707,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3375,7 +3869,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="75000"/>
@@ -3448,7 +3942,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3639,7 +4133,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3698,7 +4192,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -8302,8 +8796,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{27A9B638-6956-49FF-BB7E-7B61C43FA744}" name="数据透视表2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:B36" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{27A9B638-6956-49FF-BB7E-7B61C43FA744}" name="数据透视表2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0" measureFilter="1" sortType="descending">
@@ -8623,7 +9117,7 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="33">
+  <rowItems count="15">
     <i>
       <x v="56"/>
     </i>
@@ -8666,60 +9160,6 @@
     <i>
       <x v="5"/>
     </i>
-    <i>
-      <x v="52"/>
-    </i>
-    <i>
-      <x v="81"/>
-    </i>
-    <i>
-      <x v="50"/>
-    </i>
-    <i>
-      <x v="122"/>
-    </i>
-    <i>
-      <x v="63"/>
-    </i>
-    <i>
-      <x v="121"/>
-    </i>
-    <i>
-      <x v="110"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="57"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="61"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="67"/>
-    </i>
-    <i>
-      <x v="138"/>
-    </i>
-    <i>
-      <x v="117"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
     <i t="grand">
       <x/>
     </i>
@@ -8730,7 +9170,7 @@
   <dataFields count="1">
     <dataField name="求和项:star" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="33">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -8740,14 +9180,398 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="56"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="91"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="118"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="69"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="103"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="126"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="90"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="29"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="116"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="70"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="75"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="52"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="16">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="81"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="17">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="50"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="18">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="122"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="19">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="63"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="20">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="121"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="21">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="110"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="22">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="28"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="57"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="25">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="44"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="26">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="61"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="27">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="28">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="45"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="29">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="67"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="30">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="138"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="31">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="117"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="32">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <filters count="1">
-    <filter fld="1" type="valueGreaterThan" evalOrder="-1" id="4" iMeasureFld="0">
+    <filter fld="1" type="valueGreaterThan" evalOrder="-1" id="5" iMeasureFld="0">
       <autoFilter ref="A1">
         <filterColumn colId="0">
           <customFilters>
-            <customFilter operator="greaterThan" val="1000"/>
+            <customFilter operator="greaterThan" val="2000"/>
           </customFilters>
         </filterColumn>
       </autoFilter>
@@ -8765,7 +9589,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6BDA430A-2679-4C27-B44A-D945C82C090F}" name="数据透视表3" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6BDA430A-2679-4C27-B44A-D945C82C090F}" name="数据透视表3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A3:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0">
@@ -9378,7 +10202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF1D294-375D-424E-B79F-2BC5324DCD64}">
   <dimension ref="A1:H170"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:H170"/>
     </sheetView>
   </sheetViews>
@@ -13829,15 +14653,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC26F0B-0995-4D94-B41A-1A9BDD95C569}">
-  <dimension ref="A3:B36"/>
+  <dimension ref="A3:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="AM33" sqref="AM33"/>
+    <sheetView topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="AM7" sqref="AM7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
     <col min="3" max="40" width="3.5" bestFit="1" customWidth="1"/>
     <col min="41" max="115" width="4.5" bestFit="1" customWidth="1"/>
@@ -13968,154 +14792,10 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>64</v>
+        <v>633</v>
       </c>
       <c r="B18" s="5">
-        <v>1820</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>525</v>
-      </c>
-      <c r="B19" s="5">
-        <v>1759</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="5">
-        <v>1755</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="5">
-        <v>1742</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="5">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B23" s="5">
-        <v>1635</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="5">
-        <v>1510</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="5">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="5">
-        <v>1391</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="5">
-        <v>1255</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B28" s="5">
-        <v>1190</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B29" s="5">
-        <v>1184</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B30" s="5">
-        <v>1177</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B31" s="5">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="B32" s="5">
-        <v>1096</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B33" s="5">
-        <v>1081</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B34" s="5">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>385</v>
-      </c>
-      <c r="B35" s="5">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>633</v>
-      </c>
-      <c r="B36" s="5">
-        <v>150282</v>
+        <v>125325</v>
       </c>
     </row>
   </sheetData>
@@ -14151,7 +14831,7 @@
       <c r="A4" s="4">
         <v>2015</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
@@ -14159,7 +14839,7 @@
       <c r="A5" s="4">
         <v>2016</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5">
         <v>2</v>
       </c>
     </row>
@@ -14167,7 +14847,7 @@
       <c r="A6" s="4">
         <v>2017</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6">
         <v>5</v>
       </c>
     </row>
@@ -14175,7 +14855,7 @@
       <c r="A7" s="4">
         <v>2018</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7">
         <v>7</v>
       </c>
     </row>
@@ -14183,7 +14863,7 @@
       <c r="A8" s="4">
         <v>2019</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8">
         <v>14</v>
       </c>
     </row>
@@ -14191,7 +14871,7 @@
       <c r="A9" s="4">
         <v>2020</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9">
         <v>12</v>
       </c>
     </row>
@@ -14199,7 +14879,7 @@
       <c r="A10" s="4">
         <v>2021</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10">
         <v>14</v>
       </c>
     </row>
@@ -14207,7 +14887,7 @@
       <c r="A11" s="4">
         <v>2022</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11">
         <v>43</v>
       </c>
     </row>
@@ -14215,7 +14895,7 @@
       <c r="A12" s="4">
         <v>2023</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12">
         <v>71</v>
       </c>
     </row>
@@ -14223,7 +14903,7 @@
       <c r="A13" s="4" t="s">
         <v>633</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13">
         <v>169</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix spelling errors in uppercase and lowercase
</commit_message>
<xml_diff>
--- a/awesome_security_repo.xlsx
+++ b/awesome_security_repo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VirtualShare\awesome-cybersecurity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30736B29-3413-487A-9973-2C75F08F5C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5AE442-DEFA-4476-803B-857B176F7F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81CE6068-20D0-4AC4-A877-CDE743AA0958}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{81CE6068-20D0-4AC4-A877-CDE743AA0958}"/>
   </bookViews>
   <sheets>
     <sheet name="security" sheetId="2" r:id="rId1"/>
@@ -2012,7 +2012,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2027,9 +2027,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3688,7 +3685,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="1"/>
-              <a:t>Trend of Updated Awesome Security repositories</a:t>
+              <a:t>Trend of Updated Awesome Security Repositories</a:t>
             </a:r>
             <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1600" b="1"/>
           </a:p>
@@ -10202,7 +10199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF1D294-375D-424E-B79F-2BC5324DCD64}">
   <dimension ref="A1:H170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:H170"/>
     </sheetView>
   </sheetViews>
@@ -14655,7 +14652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC26F0B-0995-4D94-B41A-1A9BDD95C569}">
   <dimension ref="A3:B18"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
       <selection activeCell="AM7" sqref="AM7"/>
     </sheetView>
   </sheetViews>
@@ -14682,7 +14679,7 @@
       <c r="A4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4">
         <v>64822</v>
       </c>
     </row>
@@ -14690,7 +14687,7 @@
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5">
         <v>10176</v>
       </c>
     </row>
@@ -14698,7 +14695,7 @@
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6">
         <v>9780</v>
       </c>
     </row>
@@ -14706,7 +14703,7 @@
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7">
         <v>6887</v>
       </c>
     </row>
@@ -14714,7 +14711,7 @@
       <c r="A8" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8">
         <v>5897</v>
       </c>
     </row>
@@ -14722,7 +14719,7 @@
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9">
         <v>4319</v>
       </c>
     </row>
@@ -14730,7 +14727,7 @@
       <c r="A10" s="4" t="s">
         <v>612</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10">
         <v>4123</v>
       </c>
     </row>
@@ -14738,7 +14735,7 @@
       <c r="A11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11">
         <v>3803</v>
       </c>
     </row>
@@ -14746,7 +14743,7 @@
       <c r="A12" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12">
         <v>3288</v>
       </c>
     </row>
@@ -14754,7 +14751,7 @@
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13">
         <v>3047</v>
       </c>
     </row>
@@ -14762,7 +14759,7 @@
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14">
         <v>2438</v>
       </c>
     </row>
@@ -14770,7 +14767,7 @@
       <c r="A15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15">
         <v>2402</v>
       </c>
     </row>
@@ -14778,7 +14775,7 @@
       <c r="A16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16">
         <v>2204</v>
       </c>
     </row>
@@ -14786,7 +14783,7 @@
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17">
         <v>2139</v>
       </c>
     </row>
@@ -14794,7 +14791,7 @@
       <c r="A18" s="4" t="s">
         <v>633</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18">
         <v>125325</v>
       </c>
     </row>

</xml_diff>